<commit_message>
cleaned up the file a bit more
</commit_message>
<xml_diff>
--- a/Example/example_tables.xlsx
+++ b/Example/example_tables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Kirker\Documents\Git repositories\excel2latexviapython\Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repositories\excel2latexviapython\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="27840" windowHeight="13020" activeTab="2"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="27840" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="simple_table" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -169,6 +166,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="A1:D6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,29 +568,29 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -697,43 +697,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="17">
         <v>1</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="17">
         <v>2</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -753,7 +755,7 @@
       <c r="B4">
         <v>123.123</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>234.23400000000001</v>
       </c>
       <c r="D4" s="3">
@@ -775,16 +777,16 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>9</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <v>8</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Archiving current approach which works. I have a new approach which should make things easier to understand in the code. Process each cell, and output the different elements to store in different objects.
</commit_message>
<xml_diff>
--- a/Example/example_tables.xlsx
+++ b/Example/example_tables.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repositories\excel2latexviapython\Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Git Repositories\excel2latexviapython\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="27840" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="6705" yWindow="0" windowWidth="27840" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="simple_table" sheetId="1" r:id="rId1"/>
     <sheet name="merged_cells" sheetId="2" r:id="rId2"/>
-    <sheet name="styled_table" sheetId="3" r:id="rId3"/>
+    <sheet name="color" sheetId="4" r:id="rId3"/>
+    <sheet name="styled_table" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
   <si>
     <t>row label 1</t>
   </si>
@@ -71,7 +72,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,13 +96,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF907648"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -145,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -169,12 +209,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF907648"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -553,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -697,8 +750,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24">
+        <v>2</v>
+      </c>
+      <c r="D2" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26">
+        <v>5.7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.85</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>123.123</v>
+      </c>
+      <c r="C4" s="19">
+        <v>234.23400000000001</v>
+      </c>
+      <c r="D4" s="19">
+        <v>345.34500000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4">
+        <v>99</v>
+      </c>
+      <c r="D5" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25">
+        <v>9</v>
+      </c>
+      <c r="C6" s="25">
+        <v>8</v>
+      </c>
+      <c r="D6" s="25">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Code now handles color for text and cell background
</commit_message>
<xml_diff>
--- a/Example/example_tables.xlsx
+++ b/Example/example_tables.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Git Repositories\excel2latexviapython\Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Kirker\Google Drive\Git Repositories\excel2latexviapython\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6705" yWindow="0" windowWidth="27840" windowHeight="13020" activeTab="2"/>
+    <workbookView xWindow="7650" yWindow="0" windowWidth="27840" windowHeight="13020"/>
   </bookViews>
   <sheets>
-    <sheet name="simple_table" sheetId="1" r:id="rId1"/>
-    <sheet name="merged_cells" sheetId="2" r:id="rId2"/>
-    <sheet name="color" sheetId="4" r:id="rId3"/>
+    <sheet name="color" sheetId="4" r:id="rId1"/>
+    <sheet name="simple_table" sheetId="1" r:id="rId2"/>
+    <sheet name="merged_cells" sheetId="2" r:id="rId3"/>
     <sheet name="styled_table" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -206,9 +206,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -217,6 +214,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,6 +504,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="23">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23">
+        <v>2</v>
+      </c>
+      <c r="D2" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25">
+        <v>5.7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.85</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>123.123</v>
+      </c>
+      <c r="C4" s="18">
+        <v>234.23400000000001</v>
+      </c>
+      <c r="D4" s="18">
+        <v>345.34500000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4">
+        <v>99</v>
+      </c>
+      <c r="D5" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="24">
+        <v>9</v>
+      </c>
+      <c r="C6" s="24">
+        <v>8</v>
+      </c>
+      <c r="D6" s="24">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
@@ -602,7 +704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -621,15 +723,15 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="18"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="9"/>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="18"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -743,108 +845,6 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="24">
-        <v>1</v>
-      </c>
-      <c r="C2" s="24">
-        <v>2</v>
-      </c>
-      <c r="D2" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="26">
-        <v>5.7</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.85</v>
-      </c>
-      <c r="D3" s="4">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>123.123</v>
-      </c>
-      <c r="C4" s="19">
-        <v>234.23400000000001</v>
-      </c>
-      <c r="D4" s="19">
-        <v>345.34500000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4">
-        <v>99</v>
-      </c>
-      <c r="D5" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="25">
-        <v>9</v>
-      </c>
-      <c r="C6" s="25">
-        <v>8</v>
-      </c>
-      <c r="D6" s="25">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Cleaned up Readme for better instructions, moved e2lvp.py into main directory. Added new example table showing LaTeX math code
</commit_message>
<xml_diff>
--- a/Example/example_tables.xlsx
+++ b/Example/example_tables.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="0" windowWidth="27840" windowHeight="13020"/>
+    <workbookView xWindow="9540" yWindow="0" windowWidth="27840" windowHeight="13020" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="color" sheetId="4" r:id="rId1"/>
-    <sheet name="simple_table" sheetId="1" r:id="rId2"/>
+    <sheet name="simple_table" sheetId="1" r:id="rId1"/>
+    <sheet name="color" sheetId="4" r:id="rId2"/>
     <sheet name="merged_cells" sheetId="2" r:id="rId3"/>
     <sheet name="styled_table" sheetId="3" r:id="rId4"/>
+    <sheet name="calibration" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>row label 1</t>
   </si>
@@ -63,6 +64,45 @@
   </si>
   <si>
     <t>Group 2</t>
+  </si>
+  <si>
+    <t>$x$</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>$\alpha$</t>
+  </si>
+  <si>
+    <t>$\beta$</t>
+  </si>
+  <si>
+    <t>$\gamma$</t>
+  </si>
+  <si>
+    <t>$\delta$</t>
+  </si>
+  <si>
+    <t>persistence</t>
+  </si>
+  <si>
+    <t>labor share</t>
+  </si>
+  <si>
+    <t>$\sigma$</t>
+  </si>
+  <si>
+    <t>S.D. of shock</t>
+  </si>
+  <si>
+    <t>aggregate growth rate</t>
+  </si>
+  <si>
+    <t>probability of separation</t>
   </si>
 </sst>
 </file>
@@ -504,108 +544,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="23">
-        <v>1</v>
-      </c>
-      <c r="C2" s="23">
-        <v>2</v>
-      </c>
-      <c r="D2" s="23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="25">
-        <v>5.7</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.85</v>
-      </c>
-      <c r="D3" s="4">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>123.123</v>
-      </c>
-      <c r="C4" s="18">
-        <v>234.23400000000001</v>
-      </c>
-      <c r="D4" s="18">
-        <v>345.34500000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4">
-        <v>99</v>
-      </c>
-      <c r="D5" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="24">
-        <v>9</v>
-      </c>
-      <c r="C6" s="24">
-        <v>8</v>
-      </c>
-      <c r="D6" s="24">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
@@ -695,6 +633,108 @@
         <v>8</v>
       </c>
       <c r="D6" s="2">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="23">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23">
+        <v>2</v>
+      </c>
+      <c r="D2" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25">
+        <v>5.7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.85</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>123.123</v>
+      </c>
+      <c r="C4" s="18">
+        <v>234.23400000000001</v>
+      </c>
+      <c r="D4" s="18">
+        <v>345.34500000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4">
+        <v>99</v>
+      </c>
+      <c r="D5" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="24">
+        <v>9</v>
+      </c>
+      <c r="C6" s="24">
+        <v>8</v>
+      </c>
+      <c r="D6" s="24">
         <v>7</v>
       </c>
     </row>
@@ -853,7 +893,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +973,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B6" s="16">
         <v>9</v>
@@ -949,4 +989,88 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>